<commit_message>
Deploying to gh-pages from @ Healthedata1/test-stuff@01a2519fef6e2abe2bb25248827cfcf150936bea 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-treatment-intervention-preference-grouping.xlsx
+++ b/StructureDefinition-us-core-treatment-intervention-preference-grouping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2037" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2037" uniqueCount="456">
   <si>
     <t>Property</t>
   </si>
@@ -662,12 +662,6 @@
     &lt;code value="treatment-intervention-preference"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
-  </si>
-  <si>
-    <t>Codes for high level observation categories.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-category</t>
   </si>
   <si>
     <t>Observation.code</t>
@@ -3715,10 +3709,10 @@
         <v>118</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="Z16" t="s" s="2">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="AA16" t="s" s="2">
         <v>83</v>
@@ -3771,14 +3765,14 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="2">
@@ -3800,16 +3794,16 @@
         <v>192</v>
       </c>
       <c r="L17" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="M17" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="N17" t="s" s="2">
         <v>210</v>
       </c>
-      <c r="M17" t="s" s="2">
+      <c r="O17" t="s" s="2">
         <v>211</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="O17" t="s" s="2">
-        <v>213</v>
       </c>
       <c r="P17" t="s" s="2">
         <v>83</v>
@@ -3819,29 +3813,29 @@
         <v>83</v>
       </c>
       <c r="S17" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="T17" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="U17" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="V17" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="W17" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="X17" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="Y17" t="s" s="2">
         <v>214</v>
       </c>
-      <c r="T17" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="U17" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="V17" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="W17" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="X17" t="s" s="2">
+      <c r="Z17" t="s" s="2">
         <v>215</v>
       </c>
-      <c r="Y17" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="Z17" t="s" s="2">
-        <v>217</v>
-      </c>
       <c r="AA17" t="s" s="2">
         <v>83</v>
       </c>
@@ -3858,7 +3852,7 @@
         <v>83</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>94</v>
@@ -3873,30 +3867,30 @@
         <v>106</v>
       </c>
       <c r="AK17" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="AL17" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="AM17" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="AL17" t="s" s="2">
+      <c r="AN17" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="AM17" t="s" s="2">
+      <c r="AO17" t="s" s="2">
         <v>220</v>
       </c>
-      <c r="AN17" t="s" s="2">
+      <c r="AP17" t="s" s="2">
         <v>221</v>
-      </c>
-      <c r="AO17" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="AP17" t="s" s="2">
-        <v>223</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3919,19 +3913,19 @@
         <v>95</v>
       </c>
       <c r="K18" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="L18" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="M18" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="L18" t="s" s="2">
+      <c r="N18" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="M18" t="s" s="2">
+      <c r="O18" t="s" s="2">
         <v>227</v>
-      </c>
-      <c r="N18" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="O18" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="P18" t="s" s="2">
         <v>83</v>
@@ -3980,7 +3974,7 @@
         <v>83</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>81</v>
@@ -3995,19 +3989,19 @@
         <v>106</v>
       </c>
       <c r="AK18" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="AL18" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AM18" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="AN18" t="s" s="2">
         <v>230</v>
       </c>
-      <c r="AL18" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AM18" t="s" s="2">
+      <c r="AO18" t="s" s="2">
         <v>231</v>
-      </c>
-      <c r="AN18" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="AO18" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="AP18" t="s" s="2">
         <v>83</v>
@@ -4015,10 +4009,10 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -4041,16 +4035,16 @@
         <v>95</v>
       </c>
       <c r="K19" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="L19" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="M19" t="s" s="2">
         <v>235</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="N19" t="s" s="2">
         <v>236</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" t="s" s="2">
@@ -4100,7 +4094,7 @@
         <v>83</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>81</v>
@@ -4121,13 +4115,13 @@
         <v>83</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="AO19" t="s" s="2">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="AP19" t="s" s="2">
         <v>83</v>
@@ -4135,14 +4129,14 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" t="s" s="2">
@@ -4161,19 +4155,19 @@
         <v>95</v>
       </c>
       <c r="K20" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="L20" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="M20" t="s" s="2">
         <v>242</v>
       </c>
-      <c r="L20" t="s" s="2">
+      <c r="N20" t="s" s="2">
         <v>243</v>
       </c>
-      <c r="M20" t="s" s="2">
+      <c r="O20" t="s" s="2">
         <v>244</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="O20" t="s" s="2">
-        <v>246</v>
       </c>
       <c r="P20" t="s" s="2">
         <v>83</v>
@@ -4222,7 +4216,7 @@
         <v>83</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>81</v>
@@ -4237,19 +4231,19 @@
         <v>106</v>
       </c>
       <c r="AK20" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="AL20" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AM20" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="AN20" t="s" s="2">
         <v>247</v>
       </c>
-      <c r="AL20" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AM20" t="s" s="2">
+      <c r="AO20" t="s" s="2">
         <v>248</v>
-      </c>
-      <c r="AN20" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="AO20" t="s" s="2">
-        <v>250</v>
       </c>
       <c r="AP20" t="s" s="2">
         <v>83</v>
@@ -4257,14 +4251,14 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" t="s" s="2">
@@ -4283,19 +4277,19 @@
         <v>95</v>
       </c>
       <c r="K21" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="L21" t="s" s="2">
+        <v>252</v>
+      </c>
+      <c r="M21" t="s" s="2">
         <v>253</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="N21" t="s" s="2">
         <v>254</v>
       </c>
-      <c r="M21" t="s" s="2">
+      <c r="O21" t="s" s="2">
         <v>255</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="O21" t="s" s="2">
-        <v>257</v>
       </c>
       <c r="P21" t="s" s="2">
         <v>83</v>
@@ -4344,7 +4338,7 @@
         <v>83</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>81</v>
@@ -4359,19 +4353,19 @@
         <v>106</v>
       </c>
       <c r="AK21" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="AL21" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AM21" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="AN21" t="s" s="2">
         <v>258</v>
       </c>
-      <c r="AL21" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AM21" t="s" s="2">
+      <c r="AO21" t="s" s="2">
         <v>259</v>
-      </c>
-      <c r="AN21" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="AO21" t="s" s="2">
-        <v>261</v>
       </c>
       <c r="AP21" t="s" s="2">
         <v>83</v>
@@ -4379,10 +4373,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4405,16 +4399,16 @@
         <v>95</v>
       </c>
       <c r="K22" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="L22" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="M22" t="s" s="2">
         <v>263</v>
       </c>
-      <c r="L22" t="s" s="2">
+      <c r="N22" t="s" s="2">
         <v>264</v>
-      </c>
-      <c r="M22" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>266</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" t="s" s="2">
@@ -4464,7 +4458,7 @@
         <v>83</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>81</v>
@@ -4485,13 +4479,13 @@
         <v>83</v>
       </c>
       <c r="AM22" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="AN22" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="AO22" t="s" s="2">
         <v>267</v>
-      </c>
-      <c r="AN22" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="AO22" t="s" s="2">
-        <v>269</v>
       </c>
       <c r="AP22" t="s" s="2">
         <v>83</v>
@@ -4499,10 +4493,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4525,17 +4519,17 @@
         <v>95</v>
       </c>
       <c r="K23" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="L23" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="M23" t="s" s="2">
         <v>271</v>
-      </c>
-      <c r="L23" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>273</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="P23" t="s" s="2">
         <v>83</v>
@@ -4584,7 +4578,7 @@
         <v>83</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>81</v>
@@ -4599,19 +4593,19 @@
         <v>106</v>
       </c>
       <c r="AK23" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="AL23" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AM23" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AN23" t="s" s="2">
         <v>275</v>
       </c>
-      <c r="AL23" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AM23" t="s" s="2">
+      <c r="AO23" t="s" s="2">
         <v>276</v>
-      </c>
-      <c r="AN23" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="AO23" t="s" s="2">
-        <v>278</v>
       </c>
       <c r="AP23" t="s" s="2">
         <v>83</v>
@@ -4619,10 +4613,10 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4645,19 +4639,19 @@
         <v>95</v>
       </c>
       <c r="K24" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="L24" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="M24" t="s" s="2">
         <v>280</v>
       </c>
-      <c r="L24" t="s" s="2">
+      <c r="N24" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="M24" t="s" s="2">
+      <c r="O24" t="s" s="2">
         <v>282</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="O24" t="s" s="2">
-        <v>284</v>
       </c>
       <c r="P24" t="s" s="2">
         <v>83</v>
@@ -4706,7 +4700,7 @@
         <v>83</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>81</v>
@@ -4715,7 +4709,7 @@
         <v>94</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>106</v>
@@ -4724,27 +4718,27 @@
         <v>83</v>
       </c>
       <c r="AL24" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AM24" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="AN24" t="s" s="2">
         <v>286</v>
       </c>
-      <c r="AM24" t="s" s="2">
+      <c r="AO24" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AP24" t="s" s="2">
         <v>287</v>
-      </c>
-      <c r="AN24" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="AO24" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AP24" t="s" s="2">
-        <v>289</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4770,16 +4764,16 @@
         <v>192</v>
       </c>
       <c r="L25" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="M25" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="N25" t="s" s="2">
         <v>291</v>
       </c>
-      <c r="M25" t="s" s="2">
+      <c r="O25" t="s" s="2">
         <v>292</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="O25" t="s" s="2">
-        <v>294</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>83</v>
@@ -4804,14 +4798,14 @@
         <v>83</v>
       </c>
       <c r="X25" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="Y25" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="Z25" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="Y25" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="Z25" t="s" s="2">
-        <v>297</v>
-      </c>
       <c r="AA25" t="s" s="2">
         <v>83</v>
       </c>
@@ -4828,7 +4822,7 @@
         <v>83</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>81</v>
@@ -4837,7 +4831,7 @@
         <v>94</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AJ25" t="s" s="2">
         <v>106</v>
@@ -4852,7 +4846,7 @@
         <v>137</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="AO25" t="s" s="2">
         <v>83</v>
@@ -4863,14 +4857,14 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s" s="2">
@@ -4892,16 +4886,16 @@
         <v>192</v>
       </c>
       <c r="L26" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="M26" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="N26" t="s" s="2">
         <v>302</v>
       </c>
-      <c r="M26" t="s" s="2">
+      <c r="O26" t="s" s="2">
         <v>303</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>304</v>
-      </c>
-      <c r="O26" t="s" s="2">
-        <v>305</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>83</v>
@@ -4926,13 +4920,13 @@
         <v>83</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="Z26" t="s" s="2">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="AA26" t="s" s="2">
         <v>83</v>
@@ -4950,7 +4944,7 @@
         <v>83</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>81</v>
@@ -4968,27 +4962,27 @@
         <v>83</v>
       </c>
       <c r="AL26" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="AM26" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="AN26" t="s" s="2">
         <v>308</v>
       </c>
-      <c r="AM26" t="s" s="2">
+      <c r="AO26" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AP26" t="s" s="2">
         <v>309</v>
-      </c>
-      <c r="AN26" t="s" s="2">
-        <v>310</v>
-      </c>
-      <c r="AO26" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AP26" t="s" s="2">
-        <v>311</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -5011,19 +5005,19 @@
         <v>83</v>
       </c>
       <c r="K27" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="L27" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="M27" t="s" s="2">
         <v>313</v>
       </c>
-      <c r="L27" t="s" s="2">
+      <c r="N27" t="s" s="2">
         <v>314</v>
       </c>
-      <c r="M27" t="s" s="2">
+      <c r="O27" t="s" s="2">
         <v>315</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>316</v>
-      </c>
-      <c r="O27" t="s" s="2">
-        <v>317</v>
       </c>
       <c r="P27" t="s" s="2">
         <v>83</v>
@@ -5072,7 +5066,7 @@
         <v>83</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>81</v>
@@ -5093,10 +5087,10 @@
         <v>83</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AO27" t="s" s="2">
         <v>83</v>
@@ -5107,10 +5101,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -5136,13 +5130,13 @@
         <v>192</v>
       </c>
       <c r="L28" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="M28" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="N28" t="s" s="2">
         <v>321</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>323</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -5168,13 +5162,13 @@
         <v>83</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="Z28" t="s" s="2">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AA28" t="s" s="2">
         <v>83</v>
@@ -5192,7 +5186,7 @@
         <v>83</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>81</v>
@@ -5210,27 +5204,27 @@
         <v>83</v>
       </c>
       <c r="AL28" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="AM28" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="AN28" t="s" s="2">
         <v>326</v>
       </c>
-      <c r="AM28" t="s" s="2">
+      <c r="AO28" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AP28" t="s" s="2">
         <v>327</v>
-      </c>
-      <c r="AN28" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="AO28" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AP28" t="s" s="2">
-        <v>329</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5256,16 +5250,16 @@
         <v>192</v>
       </c>
       <c r="L29" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="M29" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="N29" t="s" s="2">
         <v>331</v>
       </c>
-      <c r="M29" t="s" s="2">
+      <c r="O29" t="s" s="2">
         <v>332</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>333</v>
-      </c>
-      <c r="O29" t="s" s="2">
-        <v>334</v>
       </c>
       <c r="P29" t="s" s="2">
         <v>83</v>
@@ -5290,13 +5284,13 @@
         <v>83</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="Z29" t="s" s="2">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="AA29" t="s" s="2">
         <v>83</v>
@@ -5314,7 +5308,7 @@
         <v>83</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>81</v>
@@ -5335,10 +5329,10 @@
         <v>83</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="AO29" t="s" s="2">
         <v>83</v>
@@ -5349,10 +5343,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5375,16 +5369,16 @@
         <v>83</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="L30" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="M30" t="s" s="2">
         <v>340</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="N30" t="s" s="2">
         <v>341</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>343</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -5434,7 +5428,7 @@
         <v>83</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>81</v>
@@ -5452,27 +5446,27 @@
         <v>83</v>
       </c>
       <c r="AL30" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="AM30" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="AN30" t="s" s="2">
         <v>344</v>
       </c>
-      <c r="AM30" t="s" s="2">
+      <c r="AO30" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AP30" t="s" s="2">
         <v>345</v>
-      </c>
-      <c r="AN30" t="s" s="2">
-        <v>346</v>
-      </c>
-      <c r="AO30" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AP30" t="s" s="2">
-        <v>347</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5495,16 +5489,16 @@
         <v>83</v>
       </c>
       <c r="K31" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="L31" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="M31" t="s" s="2">
         <v>349</v>
       </c>
-      <c r="L31" t="s" s="2">
+      <c r="N31" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>352</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
@@ -5554,7 +5548,7 @@
         <v>83</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>81</v>
@@ -5572,27 +5566,27 @@
         <v>83</v>
       </c>
       <c r="AL31" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="AM31" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="AN31" t="s" s="2">
         <v>353</v>
       </c>
-      <c r="AM31" t="s" s="2">
+      <c r="AO31" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AP31" t="s" s="2">
         <v>354</v>
-      </c>
-      <c r="AN31" t="s" s="2">
-        <v>355</v>
-      </c>
-      <c r="AO31" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AP31" t="s" s="2">
-        <v>356</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5615,19 +5609,19 @@
         <v>83</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="L32" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="M32" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="L32" t="s" s="2">
+      <c r="N32" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="M32" t="s" s="2">
+      <c r="O32" t="s" s="2">
         <v>360</v>
-      </c>
-      <c r="N32" t="s" s="2">
-        <v>361</v>
-      </c>
-      <c r="O32" t="s" s="2">
-        <v>362</v>
       </c>
       <c r="P32" t="s" s="2">
         <v>83</v>
@@ -5676,7 +5670,7 @@
         <v>83</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>81</v>
@@ -5688,19 +5682,19 @@
         <v>83</v>
       </c>
       <c r="AJ32" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="AK32" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AL32" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AM32" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="AN32" t="s" s="2">
         <v>363</v>
-      </c>
-      <c r="AK32" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AL32" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AM32" t="s" s="2">
-        <v>364</v>
-      </c>
-      <c r="AN32" t="s" s="2">
-        <v>365</v>
       </c>
       <c r="AO32" t="s" s="2">
         <v>83</v>
@@ -5711,10 +5705,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5737,13 +5731,13 @@
         <v>83</v>
       </c>
       <c r="K33" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="L33" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="M33" t="s" s="2">
         <v>367</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>368</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>369</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -5794,7 +5788,7 @@
         <v>83</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>81</v>
@@ -5818,7 +5812,7 @@
         <v>83</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AO33" t="s" s="2">
         <v>83</v>
@@ -5829,10 +5823,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5861,7 +5855,7 @@
         <v>141</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="N34" t="s" s="2">
         <v>143</v>
@@ -5914,7 +5908,7 @@
         <v>83</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>81</v>
@@ -5938,7 +5932,7 @@
         <v>83</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AO34" t="s" s="2">
         <v>83</v>
@@ -5949,14 +5943,14 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -5978,10 +5972,10 @@
         <v>140</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="N35" t="s" s="2">
         <v>143</v>
@@ -6036,7 +6030,7 @@
         <v>83</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>81</v>
@@ -6071,10 +6065,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -6097,13 +6091,13 @@
         <v>83</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="L36" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="M36" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>382</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>383</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -6154,7 +6148,7 @@
         <v>83</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>81</v>
@@ -6163,7 +6157,7 @@
         <v>94</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>106</v>
@@ -6175,10 +6169,10 @@
         <v>83</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="AO36" t="s" s="2">
         <v>83</v>
@@ -6189,10 +6183,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6215,13 +6209,13 @@
         <v>83</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -6272,7 +6266,7 @@
         <v>83</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>81</v>
@@ -6281,7 +6275,7 @@
         <v>94</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>106</v>
@@ -6293,10 +6287,10 @@
         <v>83</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="AO37" t="s" s="2">
         <v>83</v>
@@ -6307,10 +6301,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6336,16 +6330,16 @@
         <v>192</v>
       </c>
       <c r="L38" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="M38" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="N38" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="M38" t="s" s="2">
+      <c r="O38" t="s" s="2">
         <v>393</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>394</v>
-      </c>
-      <c r="O38" t="s" s="2">
-        <v>395</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>83</v>
@@ -6373,10 +6367,10 @@
         <v>118</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="Z38" t="s" s="2">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="AA38" t="s" s="2">
         <v>83</v>
@@ -6394,7 +6388,7 @@
         <v>83</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>81</v>
@@ -6412,13 +6406,13 @@
         <v>83</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>83</v>
@@ -6429,10 +6423,10 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6458,16 +6452,16 @@
         <v>192</v>
       </c>
       <c r="L39" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="M39" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="N39" t="s" s="2">
         <v>401</v>
       </c>
-      <c r="M39" t="s" s="2">
+      <c r="O39" t="s" s="2">
         <v>402</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>403</v>
-      </c>
-      <c r="O39" t="s" s="2">
-        <v>404</v>
       </c>
       <c r="P39" t="s" s="2">
         <v>83</v>
@@ -6492,13 +6486,13 @@
         <v>83</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="Z39" t="s" s="2">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="AA39" t="s" s="2">
         <v>83</v>
@@ -6516,7 +6510,7 @@
         <v>83</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>81</v>
@@ -6534,13 +6528,13 @@
         <v>83</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>83</v>
@@ -6551,10 +6545,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6577,17 +6571,17 @@
         <v>83</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="L40" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="M40" t="s" s="2">
         <v>408</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>409</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>410</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="P40" t="s" s="2">
         <v>83</v>
@@ -6636,7 +6630,7 @@
         <v>83</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>81</v>
@@ -6660,7 +6654,7 @@
         <v>83</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>83</v>
@@ -6671,10 +6665,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6697,13 +6691,13 @@
         <v>83</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -6754,7 +6748,7 @@
         <v>83</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>81</v>
@@ -6775,10 +6769,10 @@
         <v>83</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>83</v>
@@ -6789,10 +6783,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6815,16 +6809,16 @@
         <v>95</v>
       </c>
       <c r="K42" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="L42" t="s" s="2">
+        <v>417</v>
+      </c>
+      <c r="M42" t="s" s="2">
         <v>418</v>
       </c>
-      <c r="L42" t="s" s="2">
+      <c r="N42" t="s" s="2">
         <v>419</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>420</v>
-      </c>
-      <c r="N42" t="s" s="2">
-        <v>421</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
@@ -6874,7 +6868,7 @@
         <v>83</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>81</v>
@@ -6895,10 +6889,10 @@
         <v>83</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>83</v>
@@ -6909,10 +6903,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6935,16 +6929,16 @@
         <v>95</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="M43" t="s" s="2">
         <v>425</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>426</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>428</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
@@ -6994,7 +6988,7 @@
         <v>83</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>81</v>
@@ -7015,10 +7009,10 @@
         <v>83</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>83</v>
@@ -7029,10 +7023,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -7055,19 +7049,19 @@
         <v>95</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L44" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="N44" t="s" s="2">
         <v>431</v>
       </c>
-      <c r="M44" t="s" s="2">
+      <c r="O44" t="s" s="2">
         <v>432</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>433</v>
-      </c>
-      <c r="O44" t="s" s="2">
-        <v>434</v>
       </c>
       <c r="P44" t="s" s="2">
         <v>83</v>
@@ -7116,7 +7110,7 @@
         <v>83</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>81</v>
@@ -7137,10 +7131,10 @@
         <v>83</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>83</v>
@@ -7151,10 +7145,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7177,13 +7171,13 @@
         <v>83</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="L45" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="M45" t="s" s="2">
         <v>367</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>368</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>369</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -7234,7 +7228,7 @@
         <v>83</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>81</v>
@@ -7258,7 +7252,7 @@
         <v>83</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>83</v>
@@ -7269,10 +7263,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7301,7 +7295,7 @@
         <v>141</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="N46" t="s" s="2">
         <v>143</v>
@@ -7354,7 +7348,7 @@
         <v>83</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>81</v>
@@ -7378,7 +7372,7 @@
         <v>83</v>
       </c>
       <c r="AN46" t="s" s="2">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AO46" t="s" s="2">
         <v>83</v>
@@ -7389,14 +7383,14 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s" s="2">
@@ -7418,10 +7412,10 @@
         <v>140</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="N47" t="s" s="2">
         <v>143</v>
@@ -7476,7 +7470,7 @@
         <v>83</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>81</v>
@@ -7511,10 +7505,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7540,16 +7534,16 @@
         <v>192</v>
       </c>
       <c r="L48" t="s" s="2">
+        <v>439</v>
+      </c>
+      <c r="M48" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="N48" t="s" s="2">
         <v>441</v>
       </c>
-      <c r="M48" t="s" s="2">
-        <v>442</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>443</v>
-      </c>
       <c r="O48" t="s" s="2">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="P48" t="s" s="2">
         <v>83</v>
@@ -7574,14 +7568,14 @@
         <v>83</v>
       </c>
       <c r="X48" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="Y48" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="Z48" t="s" s="2">
         <v>215</v>
       </c>
-      <c r="Y48" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="Z48" t="s" s="2">
-        <v>217</v>
-      </c>
       <c r="AA48" t="s" s="2">
         <v>83</v>
       </c>
@@ -7598,7 +7592,7 @@
         <v>83</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>94</v>
@@ -7616,16 +7610,16 @@
         <v>83</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="AM48" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="AN48" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="AO48" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="AN48" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="AO48" t="s" s="2">
-        <v>222</v>
       </c>
       <c r="AP48" t="s" s="2">
         <v>83</v>
@@ -7633,10 +7627,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7659,19 +7653,19 @@
         <v>95</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>444</v>
+      </c>
+      <c r="L49" t="s" s="2">
+        <v>445</v>
+      </c>
+      <c r="M49" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="N49" t="s" s="2">
         <v>446</v>
       </c>
-      <c r="L49" t="s" s="2">
-        <v>447</v>
-      </c>
-      <c r="M49" t="s" s="2">
+      <c r="O49" t="s" s="2">
         <v>282</v>
-      </c>
-      <c r="N49" t="s" s="2">
-        <v>448</v>
-      </c>
-      <c r="O49" t="s" s="2">
-        <v>284</v>
       </c>
       <c r="P49" t="s" s="2">
         <v>83</v>
@@ -7720,7 +7714,7 @@
         <v>83</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>81</v>
@@ -7738,27 +7732,27 @@
         <v>83</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="AM49" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="AN49" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="AO49" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AP49" t="s" s="2">
         <v>287</v>
-      </c>
-      <c r="AN49" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="AO49" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AP49" t="s" s="2">
-        <v>289</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7784,16 +7778,16 @@
         <v>192</v>
       </c>
       <c r="L50" t="s" s="2">
+        <v>449</v>
+      </c>
+      <c r="M50" t="s" s="2">
+        <v>450</v>
+      </c>
+      <c r="N50" t="s" s="2">
         <v>451</v>
       </c>
-      <c r="M50" t="s" s="2">
-        <v>452</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>453</v>
-      </c>
       <c r="O50" t="s" s="2">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="P50" t="s" s="2">
         <v>83</v>
@@ -7818,14 +7812,14 @@
         <v>83</v>
       </c>
       <c r="X50" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="Y50" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="Z50" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="Y50" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="Z50" t="s" s="2">
-        <v>297</v>
-      </c>
       <c r="AA50" t="s" s="2">
         <v>83</v>
       </c>
@@ -7842,7 +7836,7 @@
         <v>83</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>81</v>
@@ -7851,7 +7845,7 @@
         <v>94</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>106</v>
@@ -7866,7 +7860,7 @@
         <v>137</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="AO50" t="s" s="2">
         <v>83</v>
@@ -7877,14 +7871,14 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" t="s" s="2">
@@ -7906,16 +7900,16 @@
         <v>192</v>
       </c>
       <c r="L51" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="M51" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="N51" t="s" s="2">
         <v>302</v>
       </c>
-      <c r="M51" t="s" s="2">
+      <c r="O51" t="s" s="2">
         <v>303</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>304</v>
-      </c>
-      <c r="O51" t="s" s="2">
-        <v>305</v>
       </c>
       <c r="P51" t="s" s="2">
         <v>83</v>
@@ -7940,13 +7934,13 @@
         <v>83</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="Z51" t="s" s="2">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="AA51" t="s" s="2">
         <v>83</v>
@@ -7964,7 +7958,7 @@
         <v>83</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>81</v>
@@ -7982,27 +7976,27 @@
         <v>83</v>
       </c>
       <c r="AL51" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="AM51" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="AN51" t="s" s="2">
         <v>308</v>
       </c>
-      <c r="AM51" t="s" s="2">
+      <c r="AO51" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AP51" t="s" s="2">
         <v>309</v>
-      </c>
-      <c r="AN51" t="s" s="2">
-        <v>310</v>
-      </c>
-      <c r="AO51" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AP51" t="s" s="2">
-        <v>311</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -8028,16 +8022,16 @@
         <v>84</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="O52" t="s" s="2">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="P52" t="s" s="2">
         <v>83</v>
@@ -8086,7 +8080,7 @@
         <v>83</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>81</v>
@@ -8107,10 +8101,10 @@
         <v>83</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AN52" t="s" s="2">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AO52" t="s" s="2">
         <v>83</v>

</xml_diff>